<commit_message>
[FV] Added log file and results from the long-run simulation run at IRIT cluster which took 10 days
The log file was downloaded via Filezilla to my laptop from the IRIT cluster c8ni.irit.fr and then parsed with parse_log.awk to generate the CSV file with the results, since this was not generated due to the fact that the simulation process stopped because of an assertion error.

The variance and bias were analyzed in the Excel file that had already been created for this purpose. Unfortunately, I could not analyze the variance of the integral because this information is not output to the log file...

I also slightly modified the original Excel with the analysis of variance and bias for the simulation I had run on my laptop.
</commit_message>
<xml_diff>
--- a/RL-002-QueueBlocking/results/analyze_estimates_20210627_215708_results (ANALYSIS OF VARIANCE AND BIAS).xlsx
+++ b/RL-002-QueueBlocking/results/analyze_estimates_20210627_215708_results (ANALYSIS OF VARIANCE AND BIAS).xlsx
@@ -15,10 +15,11 @@
   <definedNames>
     <definedName name="_AMO_UniqueIdentifier" hidden="1">"'3edd604e-2c72-4cf7-8df1-022d0af13fbb'"</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="12" r:id="rId5"/>
+    <pivotCache cacheId="2" r:id="rId5"/>
   </pivotCaches>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="51">
   <si>
     <t>rhos</t>
   </si>
@@ -194,9 +195,6 @@
     <t>Var(D)/E(D)^2</t>
   </si>
   <si>
-    <t>Var(I/D)</t>
-  </si>
-  <si>
     <t>log(Var(I/D))</t>
   </si>
   <si>
@@ -208,15 +206,21 @@
   <si>
     <t>Variance of FV estimator approximated by E(I)^2/E(D)^2</t>
   </si>
+  <si>
+    <t>Var(I/D) obs.</t>
+  </si>
+  <si>
+    <t>Var(I/D) appr.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="167" formatCode="0.00000%"/>
-    <numFmt numFmtId="173" formatCode="0.00000000000%"/>
-    <numFmt numFmtId="178" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.00000%"/>
+    <numFmt numFmtId="165" formatCode="0.00000000000%"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -727,12 +731,12 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -983,8 +987,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="456636288"/>
-        <c:axId val="456621056"/>
+        <c:axId val="474306048"/>
+        <c:axId val="474307968"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1160,11 +1164,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="466707200"/>
-        <c:axId val="467572992"/>
+        <c:axId val="474319488"/>
+        <c:axId val="474317952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="456636288"/>
+        <c:axId val="474306048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1186,19 +1190,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="456621056"/>
+        <c:crossAx val="474307968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="456621056"/>
+        <c:axId val="474307968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1223,12 +1226,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="456636288"/>
+        <c:crossAx val="474306048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="467572992"/>
+        <c:axId val="474317952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1252,12 +1255,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="466707200"/>
+        <c:crossAx val="474319488"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="466707200"/>
+        <c:axId val="474319488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1267,13 +1270,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="467572992"/>
+        <c:crossAx val="474317952"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -1317,7 +1320,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1493,11 +1495,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="466915712"/>
-        <c:axId val="458697344"/>
+        <c:axId val="474331392"/>
+        <c:axId val="474345472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="466915712"/>
+        <c:axId val="474331392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1507,12 +1509,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="458697344"/>
+        <c:crossAx val="474345472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="458697344"/>
+        <c:axId val="474345472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1523,14 +1525,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="466915712"/>
+        <c:crossAx val="474331392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1611,6 +1612,9 @@
       <c:pivotFmt>
         <c:idx val="1"/>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -1741,8 +1745,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="468387328"/>
-        <c:axId val="468388864"/>
+        <c:axId val="475249664"/>
+        <c:axId val="475260032"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1814,11 +1818,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="479882240"/>
-        <c:axId val="479879552"/>
+        <c:axId val="475267456"/>
+        <c:axId val="475261568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="468387328"/>
+        <c:axId val="475249664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1840,13 +1844,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="468388864"/>
+        <c:crossAx val="475260032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1854,7 +1857,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="468388864"/>
+        <c:axId val="475260032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1878,12 +1881,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="468387328"/>
+        <c:crossAx val="475249664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="479879552"/>
+        <c:axId val="475261568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1907,12 +1910,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="479882240"/>
+        <c:crossAx val="475267456"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="479882240"/>
+        <c:axId val="475267456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1921,7 +1924,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="479879552"/>
+        <c:crossAx val="475261568"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1936,7 +1940,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2211,11 +2214,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="486263808"/>
-        <c:axId val="486269696"/>
+        <c:axId val="475298048"/>
+        <c:axId val="475300224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="486263808"/>
+        <c:axId val="475298048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2237,14 +2240,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="486269696"/>
+        <c:crossAx val="475300224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2252,7 +2254,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="486269696"/>
+        <c:axId val="475300224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2275,21 +2277,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="486263808"/>
+        <c:crossAx val="475298048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2318,9 +2318,54 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200"/>
+              <a:t>Approximation of Var(I/D) </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" b="0"/>
+              <a:t>~ E(I)^2</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" b="0" baseline="0"/>
+              <a:t>/E(D)^2</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1200" b="0"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.20035033999483517"/>
+          <c:y val="2.7777777777777776E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13683329925144458"/>
+          <c:y val="0.17218759113444151"/>
+          <c:w val="0.55546909226349173"/>
+          <c:h val="0.70649278215223099"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -2338,6 +2383,27 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Analysis Sq. Expected'!$F$5:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Analysis Sq. Expected'!$G$5:$G$8</c:f>
@@ -2355,6 +2421,64 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2.1386343718198555E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Analysis Sq. Expected'!$H$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>E(D)^2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Analysis Sq. Expected'!$F$5:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Analysis Sq. Expected'!$H$5:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>146.95265377781405</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16701.563394369772</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>171978.35854417499</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1829557.8228784564</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2371,43 +2495,118 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="482452992"/>
-        <c:axId val="482474240"/>
+        <c:axId val="475513216"/>
+        <c:axId val="475515520"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:idx val="2"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Analysis Sq. Expected'!$H$4</c:f>
+              <c:f>'Analysis Sq. Expected'!$O$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>E(D)^2</c:v>
+                  <c:v>Var(I/D) appr.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:val>
+          <c:cat>
             <c:numRef>
-              <c:f>'Analysis Sq. Expected'!$H$5:$H$8</c:f>
+              <c:f>'Analysis Sq. Expected'!$F$5:$F$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>146.95265377781405</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16701.563394369772</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>171978.35854417499</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1829557.8228784564</c:v>
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Analysis Sq. Expected'!$O$5:$O$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.7232902549967021E-12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.7317098145156996E-11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3733818216064671E-11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1689351082957994E-11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Analysis Sq. Expected'!$Q$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Var(I/D) obs.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="92D050"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Analysis Sq. Expected'!$Q$5:$Q$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>6.8137450960310296E-12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.0194315988209423E-12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7811533070551939E-12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2675178487843402E-12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2424,20 +2623,47 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="458852992"/>
-        <c:axId val="458850688"/>
+        <c:axId val="475523712"/>
+        <c:axId val="475521792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="482452992"/>
+        <c:axId val="475513216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>J as fraction of K</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.3548818730923689"/>
+              <c:y val="0.89256926217556143"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="482474240"/>
+        <c:crossAx val="475515520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2445,47 +2671,124 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="482474240"/>
+        <c:axId val="475515520"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>log scale</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="3.0630630941037414E-2"/>
+              <c:y val="8.2829542140565759E-2"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="482452992"/>
+        <c:crossAx val="475513216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="458850688"/>
+        <c:axId val="475521792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr>
+                    <a:solidFill>
+                      <a:srgbClr val="92D050"/>
+                    </a:solidFill>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:solidFill>
+                      <a:srgbClr val="92D050"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>log scale</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.70907447085068209"/>
+              <c:y val="5.5051764362787983E-2"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="458852992"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="1">
+                <a:solidFill>
+                  <a:srgbClr val="92D050"/>
+                </a:solidFill>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="475523712"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="458852992"/>
+        <c:axId val="475523712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="458850688"/>
+        <c:crossAx val="475521792"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2552,7 +2855,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.2111111111111122E-2"/>
+          <c:x val="0.15211111111111114"/>
           <c:y val="2.7777777777777776E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -2560,7 +2863,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14259951881014873"/>
+          <c:y val="0.16089129483814524"/>
+          <c:w val="0.66753915135608044"/>
+          <c:h val="0.71778907844852724"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -2578,6 +2891,27 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Analysis Sq. Expected'!$F$5:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Analysis Sq. Expected'!$I$5:$I$8</c:f>
@@ -2615,6 +2949,27 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Analysis Sq. Expected'!$F$5:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Analysis Sq. Expected'!$G$5:$G$8</c:f>
@@ -2652,6 +3007,27 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Analysis Sq. Expected'!$F$5:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Analysis Sq. Expected'!$J$5:$J$8</c:f>
@@ -2689,6 +3065,31 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Analysis Sq. Expected'!$F$5:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Analysis Sq. Expected'!$H$5:$H$8</c:f>
@@ -2722,20 +3123,47 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="508793216"/>
-        <c:axId val="508794752"/>
+        <c:axId val="475427584"/>
+        <c:axId val="475429504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="508793216"/>
+        <c:axId val="475427584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>J as fraction of K</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.37556364829396327"/>
+              <c:y val="0.88793963254593178"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="508794752"/>
+        <c:crossAx val="475429504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2743,7 +3171,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="508794752"/>
+        <c:axId val="475429504"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2751,11 +3179,37 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>log scale</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.9444444444444445E-2"/>
+              <c:y val="7.7181393992417621E-2"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="508793216"/>
+        <c:crossAx val="475427584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2916,14 +3370,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>123265</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>347383</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>186017</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>246530</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>683559</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>71717</xdr:rowOff>
     </xdr:to>
@@ -2993,7 +3447,7 @@
         <n v="0.6"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="Pr(FV)" numFmtId="167">
+    <cacheField name="Pr(FV)" numFmtId="164">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="2.9691631560160601E-7" maxValue="8.87977672060307E-6"/>
     </cacheField>
     <cacheField name="integral" numFmtId="0">
@@ -3002,10 +3456,10 @@
     <cacheField name="E(T)" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="11.1575386961813" maxValue="1488.0032852869999"/>
     </cacheField>
-    <cacheField name="BIAS" numFmtId="167">
+    <cacheField name="BIAS" numFmtId="164">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-3.6427076917851736E-6" maxValue="4.9401527132162903E-6"/>
     </cacheField>
-    <cacheField name="BIAS2" numFmtId="173">
+    <cacheField name="BIAS2" numFmtId="165">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="6.6880651761678302E-14" maxValue="2.4405108829898275E-11"/>
     </cacheField>
   </cacheFields>
@@ -3183,7 +3637,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" chartFormat="17">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" chartFormat="17">
   <location ref="A3:D9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
@@ -3195,11 +3649,11 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField dataField="1" compact="0" numFmtId="167" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" numFmtId="164" outline="0" showAll="0"/>
     <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
     <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" numFmtId="167" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" numFmtId="173" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" numFmtId="164" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" numFmtId="165" outline="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="0"/>
@@ -3279,7 +3733,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" chartFormat="18">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" chartFormat="18">
   <location ref="A3:D9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
@@ -3291,11 +3745,11 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField dataField="1" compact="0" numFmtId="167" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" numFmtId="164" outline="0" showAll="0"/>
     <pivotField compact="0" outline="0" showAll="0"/>
     <pivotField compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" numFmtId="167" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" compact="0" numFmtId="173" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" numFmtId="164" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" compact="0" numFmtId="165" outline="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="0"/>
@@ -3375,7 +3829,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" chartFormat="23">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0" chartFormat="23">
   <location ref="A3:D9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
@@ -3387,11 +3841,11 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField dataField="1" compact="0" numFmtId="167" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" numFmtId="164" outline="0" showAll="0"/>
     <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
     <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
-    <pivotField compact="0" numFmtId="167" outline="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField compact="0" numFmtId="173" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" numFmtId="164" outline="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField compact="0" numFmtId="165" outline="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="1">
     <field x="0"/>
@@ -3432,7 +3886,7 @@
     <dataField name="Average of E0(T_A)" fld="3" subtotal="average" baseField="0" baseItem="0"/>
     <dataField name="Average of Pr(FV)" fld="1" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="6">
+  <chartFormats count="3">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -3452,33 +3906,6 @@
       </pivotArea>
     </chartFormat>
     <chartFormat chart="0" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="17" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="17" format="3" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="17" format="4" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -5344,7 +5771,7 @@
         <v>1.3330913847253966E-6</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6:F8" si="0">E6^2</f>
+        <f>E6^2</f>
         <v>1.7771326400290753E-12</v>
       </c>
       <c r="H6">
@@ -5358,7 +5785,7 @@
         <v>1.7771326400290753E-12</v>
       </c>
       <c r="K6">
-        <f t="shared" ref="K6:K8" si="1">I6+J6</f>
+        <f>I6+J6</f>
         <v>8.7965642388500176E-12</v>
       </c>
       <c r="L6">
@@ -5387,7 +5814,7 @@
         <v>-2.6668066511871758E-7</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
+        <f>E7^2</f>
         <v>7.1118577148161585E-14</v>
       </c>
       <c r="H7">
@@ -5401,7 +5828,7 @@
         <v>7.1118577148161585E-14</v>
       </c>
       <c r="K7">
-        <f t="shared" si="1"/>
+        <f>I7+J7</f>
         <v>1.8522718842033553E-12</v>
       </c>
       <c r="L7">
@@ -5430,7 +5857,7 @@
         <v>-5.6420798788619202E-7</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
+        <f>E8^2</f>
         <v>3.1833065359458539E-13</v>
       </c>
       <c r="H8">
@@ -5444,7 +5871,7 @@
         <v>3.1833065359458539E-13</v>
       </c>
       <c r="K8">
-        <f t="shared" si="1"/>
+        <f>I8+J8</f>
         <v>1.5858485023789255E-12</v>
       </c>
       <c r="L8">
@@ -5477,10 +5904,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:P9"/>
+  <dimension ref="A3:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5498,17 +5925,18 @@
     <col min="13" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>27</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -5546,19 +5974,22 @@
         <v>44</v>
       </c>
       <c r="M4" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="N4" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="N4" s="8" t="s">
-        <v>48</v>
-      </c>
       <c r="O4" t="s">
+        <v>50</v>
+      </c>
+      <c r="P4" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="P4" s="8" t="s">
-        <v>46</v>
+      <c r="Q4" s="8" t="s">
+        <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.2</v>
       </c>
@@ -5604,11 +6035,11 @@
         <v>4.6091224141232489E-3</v>
       </c>
       <c r="M5" s="8">
-        <f>LOG10(K5)</f>
+        <f t="shared" ref="M5:N8" si="0">LOG10(K5)</f>
         <v>0.25737204714106066</v>
       </c>
       <c r="N5" s="8">
-        <f t="shared" ref="N5:N8" si="0">LOG10(L5)</f>
+        <f t="shared" si="0"/>
         <v>-2.3363817572536014</v>
       </c>
       <c r="O5" s="10">
@@ -5619,8 +6050,12 @@
         <f>LOG10(O5)</f>
         <v>-11.429073106346788</v>
       </c>
+      <c r="Q5">
+        <f>GETPIVOTDATA("Variance of Pr(FV)",'Analysis Variance &amp; Bias'!$A$3,"buffer_size_activation",'Analysis Variance &amp; Bias'!$A5)</f>
+        <v>6.8137450960310296E-12</v>
+      </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.4</v>
       </c>
@@ -5638,15 +6073,15 @@
         <v>5.2265761398029009E-6</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6:F9" si="1">A6</f>
+        <f>A6</f>
         <v>0.4</v>
       </c>
       <c r="G6">
-        <f t="shared" ref="G6:G8" si="2">GETPIVOTDATA("Average of Integral",$A$3,"buffer_size_activation",$A6)^2</f>
+        <f>GETPIVOTDATA("Average of Integral",$A$3,"buffer_size_activation",$A6)^2</f>
         <v>4.5623824642156047E-7</v>
       </c>
       <c r="H6">
-        <f t="shared" ref="H6:H8" si="3">GETPIVOTDATA("Average of E0(T_A)",$A$3,"buffer_size_activation",$A6)^2</f>
+        <f>GETPIVOTDATA("Average of E0(T_A)",$A$3,"buffer_size_activation",$A6)^2</f>
         <v>16701.563394369772</v>
       </c>
       <c r="I6">
@@ -5658,15 +6093,15 @@
         <v>98.31375089479377</v>
       </c>
       <c r="K6" s="7">
-        <f t="shared" ref="K6:L8" si="4">I6/G6</f>
+        <f t="shared" ref="K6:L8" si="1">I6/G6</f>
         <v>0.26910668420757528</v>
       </c>
       <c r="L6" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>5.8864998786841783E-3</v>
       </c>
       <c r="M6" s="8">
-        <f t="shared" ref="M6:M8" si="5">LOG10(K6)</f>
+        <f t="shared" si="0"/>
         <v>-0.57007551487684927</v>
       </c>
       <c r="N6" s="8">
@@ -5674,15 +6109,19 @@
         <v>-2.2301428605958851</v>
       </c>
       <c r="O6">
-        <f t="shared" ref="O6:O9" si="6">G6/H6</f>
+        <f>G6/H6</f>
         <v>2.7317098145156996E-11</v>
       </c>
       <c r="P6" s="8">
-        <f t="shared" ref="P6:P9" si="7">LOG10(O6)</f>
+        <f>LOG10(O6)</f>
         <v>-10.563565436999326</v>
       </c>
+      <c r="Q6">
+        <f>GETPIVOTDATA("Variance of Pr(FV)",'Analysis Variance &amp; Bias'!$A$3,"buffer_size_activation",'Analysis Variance &amp; Bias'!$A6)</f>
+        <v>7.0194315988209423E-12</v>
+      </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.5</v>
       </c>
@@ -5700,15 +6139,15 @@
         <v>3.7059166499079106E-6</v>
       </c>
       <c r="F7">
-        <f t="shared" si="1"/>
+        <f>A7</f>
         <v>0.5</v>
       </c>
       <c r="G7">
-        <f t="shared" si="2"/>
+        <f>GETPIVOTDATA("Average of Integral",$A$3,"buffer_size_activation",$A7)^2</f>
         <v>2.3619195133428918E-6</v>
       </c>
       <c r="H7">
-        <f t="shared" si="3"/>
+        <f>GETPIVOTDATA("Average of E0(T_A)",$A$3,"buffer_size_activation",$A7)^2</f>
         <v>171978.35854417499</v>
       </c>
       <c r="I7">
@@ -5720,15 +6159,15 @@
         <v>343.55928760088977</v>
       </c>
       <c r="K7" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>0.15290509154027679</v>
       </c>
       <c r="L7" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1.9976890726785363E-3</v>
       </c>
       <c r="M7" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>-0.81557805290664209</v>
       </c>
       <c r="N7" s="8">
@@ -5736,15 +6175,19 @@
         <v>-2.6994721059639022</v>
       </c>
       <c r="O7">
-        <f t="shared" si="6"/>
+        <f>G7/H7</f>
         <v>1.3733818216064671E-11</v>
       </c>
       <c r="P7" s="8">
-        <f t="shared" si="7"/>
+        <f>LOG10(O7)</f>
         <v>-10.862208705324113</v>
       </c>
+      <c r="Q7">
+        <f>GETPIVOTDATA("Variance of Pr(FV)",'Analysis Variance &amp; Bias'!$A$3,"buffer_size_activation",'Analysis Variance &amp; Bias'!$A7)</f>
+        <v>1.7811533070551939E-12</v>
+      </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.6</v>
       </c>
@@ -5762,15 +6205,15 @@
         <v>3.4189693012599567E-6</v>
       </c>
       <c r="F8">
-        <f t="shared" si="1"/>
+        <f>A8</f>
         <v>0.6</v>
       </c>
       <c r="G8">
-        <f t="shared" si="2"/>
+        <f>GETPIVOTDATA("Average of Integral",$A$3,"buffer_size_activation",$A8)^2</f>
         <v>2.1386343718198555E-5</v>
       </c>
       <c r="H8">
-        <f t="shared" si="3"/>
+        <f>GETPIVOTDATA("Average of E0(T_A)",$A$3,"buffer_size_activation",$A8)^2</f>
         <v>1829557.8228784564</v>
       </c>
       <c r="I8">
@@ -5782,15 +6225,15 @@
         <v>7764.2073899704219</v>
       </c>
       <c r="K8" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>0.14531680568018154</v>
       </c>
       <c r="L8" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>4.2437616854081924E-3</v>
       </c>
       <c r="M8" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="0"/>
         <v>-0.83768415726347834</v>
       </c>
       <c r="N8" s="8">
@@ -5798,15 +6241,19 @@
         <v>-2.3722490125223898</v>
       </c>
       <c r="O8">
-        <f t="shared" si="6"/>
+        <f>G8/H8</f>
         <v>1.1689351082957994E-11</v>
       </c>
       <c r="P8" s="8">
-        <f t="shared" si="7"/>
+        <f>LOG10(O8)</f>
         <v>-10.932209597385025</v>
       </c>
+      <c r="Q8">
+        <f>GETPIVOTDATA("Variance of Pr(FV)",'Analysis Variance &amp; Bias'!$A$3,"buffer_size_activation",'Analysis Variance &amp; Bias'!$A8)</f>
+        <v>1.2675178487843402E-12</v>
+      </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>

</xml_diff>